<commit_message>
Excel sheet newly added
</commit_message>
<xml_diff>
--- a/整理.xlsx
+++ b/整理.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="追加" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>＃</t>
     <phoneticPr fontId="1"/>
@@ -101,6 +102,30 @@
     </rPh>
     <rPh sb="19" eb="21">
       <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>もう一度、修正</t>
+    <rPh sb="2" eb="4">
+      <t>イチド</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シート追加</t>
+    <rPh sb="3" eb="5">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここに追加</t>
+    <rPh sb="3" eb="5">
+      <t>ツイカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -470,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -536,9 +561,15 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -693,4 +724,26 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>